<commit_message>
add zutnlp_text Logs and frameworks
</commit_message>
<xml_diff>
--- a/zutnlp-master/zutnlp-text/doc/log/支友盟.xlsx
+++ b/zutnlp-master/zutnlp-text/doc/log/支友盟.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36">
   <si>
     <t>日志报告</t>
   </si>
@@ -113,17 +113,6 @@
   </si>
   <si>
     <t>2018.07.21</t>
-  </si>
-  <si>
-    <t>小组内统一配置完成环境，并共同商量解决每一个人的问题</t>
-  </si>
-  <si>
-    <t>小组成员环境配置完
-成，例子全部实现</t>
-  </si>
-  <si>
-    <t>Spring Boot 不能放
-置到Maven项目里面</t>
   </si>
   <si>
     <t>2018.07.22</t>
@@ -191,6 +180,97 @@
       <scheme val="major"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -201,6 +281,36 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,127 +323,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -344,31 +333,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,13 +483,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -398,133 +513,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,11 +529,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -559,16 +546,31 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -590,24 +592,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -620,21 +624,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -643,10 +632,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -655,133 +644,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1125,8 +1114,8 @@
   <sheetPr/>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -1219,78 +1208,69 @@
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" ht="47" customHeight="1" spans="1:4">
+    <row r="8" ht="30" customHeight="1" spans="1:1">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="9" ht="30" customHeight="1" spans="1:1">
       <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1" spans="1:1">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" ht="30" customHeight="1" spans="1:1">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" ht="30" customHeight="1" spans="1:1">
       <c r="A12" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" ht="30" customHeight="1" spans="1:1">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" ht="30" customHeight="1" spans="1:1">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" ht="30" customHeight="1" spans="1:1">
       <c r="A15" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>